<commit_message>
remove ovsapp in each server to constant
</commit_message>
<xml_diff>
--- a/data/workload.xlsx
+++ b/data/workload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nightraven/Coding/optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA14CAD-26A0-DC44-9B70-9D0024573B0F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664351BE-3358-5042-ADFF-9C2193E51598}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="940" windowWidth="27640" windowHeight="15820" activeTab="1" xr2:uid="{8F198691-3026-7942-A2C4-D9F6FECBD38E}"/>
+    <workbookView xWindow="1160" yWindow="940" windowWidth="27640" windowHeight="15820" xr2:uid="{8F198691-3026-7942-A2C4-D9F6FECBD38E}"/>
   </bookViews>
   <sheets>
     <sheet name="DC1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="116">
   <si>
     <t>id</t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>48730f97-5089-4729-9580-0b2b86e41562</t>
-  </si>
-  <si>
-    <t>ovsapp</t>
   </si>
   <si>
     <t>gsbmymohqapp01</t>
@@ -804,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF88E40E-0C56-8F4D-A1B4-15912409B547}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -815,7 +812,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1103,18 +1100,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18">
-        <v>3.944</v>
-      </c>
-      <c r="D18">
-        <v>3.9889999999999999</v>
-      </c>
-      <c r="E18">
-        <v>4.1289999999999996</v>
-      </c>
+      <c r="A18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1125,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A3671C-999B-8048-9754-A6AB011C612A}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:E15"/>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1136,7 +1122,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1153,10 +1139,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C2">
         <v>5.4409999999999998</v>
@@ -1170,10 +1156,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="C3">
         <v>0.42499999999999999</v>
@@ -1187,10 +1173,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="C4">
         <v>0.11600000000000001</v>
@@ -1204,10 +1190,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="C5">
         <v>0.99299999999999999</v>
@@ -1221,10 +1207,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="C6">
         <v>0.61899999999999999</v>
@@ -1238,10 +1224,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="C7">
         <v>2.7090000000000001</v>
@@ -1255,10 +1241,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="C8">
         <v>5.1999999999999998E-2</v>
@@ -1272,10 +1258,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="C9">
         <v>0.61899999999999999</v>
@@ -1289,10 +1275,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C10">
         <v>1.0469999999999999</v>
@@ -1306,10 +1292,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="C11">
         <v>1.9E-2</v>
@@ -1323,10 +1309,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1340,10 +1326,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="C13">
         <v>0.46600000000000003</v>
@@ -1357,10 +1343,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1373,18 +1359,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15">
-        <v>3.911</v>
-      </c>
-      <c r="D15">
-        <v>3.823</v>
-      </c>
-      <c r="E15">
-        <v>3.8079999999999998</v>
-      </c>
+      <c r="A15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1396,14 +1371,14 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A14" sqref="A14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1420,10 +1395,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>59</v>
       </c>
       <c r="C2">
         <v>6.0000000000000001E-3</v>
@@ -1437,10 +1412,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="C3">
         <v>0.437</v>
@@ -1454,10 +1429,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="C4">
         <v>8.3789999999999996</v>
@@ -1471,10 +1446,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C5">
         <v>0.29499999999999998</v>
@@ -1488,10 +1463,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="C6">
         <v>0.31</v>
@@ -1505,10 +1480,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="C7">
         <v>6.3730000000000002</v>
@@ -1522,10 +1497,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="C8">
         <v>4.5999999999999999E-2</v>
@@ -1539,10 +1514,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C9">
         <v>3.7999999999999999E-2</v>
@@ -1556,10 +1531,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="C10">
         <v>4.9000000000000002E-2</v>
@@ -1573,10 +1548,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1590,10 +1565,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="C12">
         <v>1.3029999999999999</v>
@@ -1607,10 +1582,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="C13">
         <v>5.7000000000000002E-2</v>
@@ -1623,18 +1598,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14">
-        <v>1.6060000000000001</v>
-      </c>
-      <c r="D14">
-        <v>1.74</v>
-      </c>
-      <c r="E14">
-        <v>1.149</v>
-      </c>
+      <c r="A14" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1646,7 +1610,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:E9"/>
+      <selection activeCell="A18" sqref="A18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1656,7 +1620,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1673,10 +1637,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="C2">
         <v>5.2069999999999999</v>
@@ -1690,10 +1654,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="C3">
         <v>0.41599999999999998</v>
@@ -1707,10 +1671,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="C4">
         <v>0.23300000000000001</v>
@@ -1724,10 +1688,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="C5">
         <v>4.9000000000000002E-2</v>
@@ -1741,10 +1705,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="C6">
         <v>2.11</v>
@@ -1758,10 +1722,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="C7">
         <v>2.9000000000000001E-2</v>
@@ -1775,10 +1739,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="C8">
         <v>0.20599999999999999</v>
@@ -1792,10 +1756,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>96</v>
       </c>
       <c r="C9">
         <v>3.722</v>
@@ -1809,10 +1773,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>98</v>
       </c>
       <c r="C10">
         <v>2.9990000000000001</v>
@@ -1826,10 +1790,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="C11">
         <v>0.60799999999999998</v>
@@ -1843,10 +1807,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="C12">
         <v>9.1999999999999998E-2</v>
@@ -1860,10 +1824,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="C13">
         <v>0.47099999999999997</v>
@@ -1877,10 +1841,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="C14">
         <v>0.41199999999999998</v>
@@ -1894,10 +1858,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="C15">
         <v>0.41399999999999998</v>
@@ -1911,10 +1875,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="C16">
         <v>4.032</v>
@@ -1928,10 +1892,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="C17">
         <v>2.1000000000000001E-2</v>
@@ -1944,18 +1908,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18">
-        <v>2.2080000000000002</v>
-      </c>
-      <c r="D18">
-        <v>2.6779999999999999</v>
-      </c>
-      <c r="E18">
-        <v>1.8879999999999999</v>
-      </c>
+      <c r="A18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sort data in workload.xlsx
</commit_message>
<xml_diff>
--- a/data/workload.xlsx
+++ b/data/workload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nightraven/Coding/optimization/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nightraven/Working/Optimization/code/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664351BE-3358-5042-ADFF-9C2193E51598}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C231D54-B02B-8940-BF45-EE16AD63EB59}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="940" windowWidth="27640" windowHeight="15820" xr2:uid="{8F198691-3026-7942-A2C4-D9F6FECBD38E}"/>
+    <workbookView xWindow="12060" yWindow="680" windowWidth="27640" windowHeight="15820" xr2:uid="{8F198691-3026-7942-A2C4-D9F6FECBD38E}"/>
   </bookViews>
   <sheets>
     <sheet name="DC1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="DC3" sheetId="3" r:id="rId3"/>
     <sheet name="DC4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -467,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -485,6 +485,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF88E40E-0C56-8F4D-A1B4-15912409B547}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:E18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -829,280 +833,283 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="C2">
-        <v>0.74199999999999999</v>
+        <v>2.056</v>
       </c>
       <c r="D2">
-        <v>0.53100000000000003</v>
+        <v>2.0960000000000001</v>
       </c>
       <c r="E2">
-        <v>0.97</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C3">
-        <v>0.64900000000000002</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="D3">
-        <v>0.97</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="E3">
-        <v>0.79800000000000004</v>
+        <v>0.13600000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C4">
-        <v>0.57899999999999996</v>
+        <v>0.72799999999999998</v>
       </c>
       <c r="D4">
-        <v>0.96299999999999997</v>
+        <v>0.73</v>
       </c>
       <c r="E4">
-        <v>0.81699999999999995</v>
+        <v>0.75900000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C5">
-        <v>9.2999999999999999E-2</v>
+        <v>0.125</v>
       </c>
       <c r="D5">
-        <v>6.4000000000000001E-2</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="E5">
-        <v>7.8E-2</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C6">
-        <v>2.4E-2</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="D6">
-        <v>2.3E-2</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="E6">
-        <v>2.1999999999999999E-2</v>
+        <v>0.11899999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C7">
-        <v>1.306</v>
+        <v>0.125</v>
       </c>
       <c r="D7">
-        <v>0.96399999999999997</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="E7">
-        <v>1.135</v>
+        <v>0.13800000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>0.52200000000000002</v>
+        <v>0.74199999999999999</v>
       </c>
       <c r="D8">
-        <v>0.34399999999999997</v>
+        <v>0.53100000000000003</v>
       </c>
       <c r="E8">
-        <v>0.34200000000000003</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>0.10299999999999999</v>
+        <v>0.64900000000000002</v>
       </c>
       <c r="D9">
-        <v>8.4000000000000005E-2</v>
+        <v>0.97</v>
       </c>
       <c r="E9">
-        <v>0.13600000000000001</v>
+        <v>0.79800000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C10">
-        <v>0.47799999999999998</v>
+        <v>0.57899999999999996</v>
       </c>
       <c r="D10">
-        <v>0.60599999999999998</v>
+        <v>0.96299999999999997</v>
       </c>
       <c r="E10">
-        <v>0.51100000000000001</v>
+        <v>0.81699999999999995</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11">
-        <v>0.22700000000000001</v>
+        <v>0.47799999999999998</v>
       </c>
       <c r="D11">
-        <v>0.26</v>
+        <v>0.60599999999999998</v>
       </c>
       <c r="E11">
-        <v>0.188</v>
+        <v>0.51100000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12">
-        <v>0.22</v>
+        <v>0.22700000000000001</v>
       </c>
       <c r="D12">
-        <v>0.159</v>
+        <v>0.26</v>
       </c>
       <c r="E12">
-        <v>0.19600000000000001</v>
+        <v>0.188</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13">
-        <v>0.72799999999999998</v>
+        <v>0.22</v>
       </c>
       <c r="D13">
-        <v>0.73</v>
+        <v>0.159</v>
       </c>
       <c r="E13">
-        <v>0.75900000000000001</v>
+        <v>0.19600000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C14">
-        <v>0.125</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="D14">
-        <v>0.10299999999999999</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="E14">
-        <v>0.09</v>
+        <v>7.8E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C15">
-        <v>0.16400000000000001</v>
+        <v>2.4E-2</v>
       </c>
       <c r="D15">
-        <v>0.19900000000000001</v>
+        <v>2.3E-2</v>
       </c>
       <c r="E15">
-        <v>0.11899999999999999</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C16">
-        <v>0.125</v>
+        <v>1.306</v>
       </c>
       <c r="D16">
-        <v>0.13400000000000001</v>
+        <v>0.96399999999999997</v>
       </c>
       <c r="E16">
-        <v>0.13800000000000001</v>
+        <v>1.135</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C17">
-        <v>2.056</v>
+        <v>0.52200000000000002</v>
       </c>
       <c r="D17">
-        <v>2.0960000000000001</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="E17">
-        <v>2.13</v>
+        <v>0.34200000000000003</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
     </row>
   </sheetData>
+  <sortState ref="A2:E17">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1111,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A3671C-999B-8048-9754-A6AB011C612A}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:E15"/>
+    <sheetView topLeftCell="A2" zoomScale="139" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1139,206 +1146,206 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C2">
-        <v>5.4409999999999998</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="D2">
-        <v>7.8739999999999997</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="E2">
-        <v>4.758</v>
+        <v>5.7000000000000002E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C3">
-        <v>0.42499999999999999</v>
+        <v>0.61899999999999999</v>
       </c>
       <c r="D3">
-        <v>0.44</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="E3">
-        <v>2.0739999999999998</v>
+        <v>0.61599999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>38</v>
+      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C4">
-        <v>0.11600000000000001</v>
+        <v>5.4409999999999998</v>
       </c>
       <c r="D4">
-        <v>9.9000000000000005E-2</v>
+        <v>7.8739999999999997</v>
       </c>
       <c r="E4">
-        <v>0.121</v>
+        <v>4.758</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C5">
-        <v>0.99299999999999999</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="D5">
-        <v>0.69199999999999995</v>
+        <v>0.44</v>
       </c>
       <c r="E5">
-        <v>1.0609999999999999</v>
+        <v>2.0739999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>42</v>
+      <c r="A6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="C6">
-        <v>0.61899999999999999</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="D6">
-        <v>0.55700000000000005</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="E6">
-        <v>0.70599999999999996</v>
+        <v>0.121</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C7">
-        <v>2.7090000000000001</v>
+        <v>0.99299999999999999</v>
       </c>
       <c r="D7">
-        <v>2.2040000000000002</v>
+        <v>0.69199999999999995</v>
       </c>
       <c r="E7">
-        <v>3.3140000000000001</v>
+        <v>1.0609999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C8">
-        <v>5.1999999999999998E-2</v>
+        <v>0.61899999999999999</v>
       </c>
       <c r="D8">
-        <v>6.4000000000000001E-2</v>
+        <v>0.55700000000000005</v>
       </c>
       <c r="E8">
-        <v>5.7000000000000002E-2</v>
+        <v>0.70599999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C9">
-        <v>0.61899999999999999</v>
+        <v>1.0469999999999999</v>
       </c>
       <c r="D9">
-        <v>0.56999999999999995</v>
+        <v>0.93100000000000005</v>
       </c>
       <c r="E9">
-        <v>0.61599999999999999</v>
+        <v>1.016</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C10">
-        <v>1.0469999999999999</v>
+        <v>1.9E-2</v>
       </c>
       <c r="D10">
-        <v>0.93100000000000005</v>
+        <v>0.02</v>
       </c>
       <c r="E10">
-        <v>1.016</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C11">
-        <v>1.9E-2</v>
+        <v>2.7090000000000001</v>
       </c>
       <c r="D11">
-        <v>0.02</v>
+        <v>2.2040000000000002</v>
       </c>
       <c r="E11">
-        <v>2.3E-2</v>
+        <v>3.3140000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>113</v>
+        <v>54</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="D12">
-        <v>1.4E-2</v>
+        <v>0.22800000000000001</v>
       </c>
       <c r="E12">
-        <v>1.0999999999999999E-2</v>
+        <v>0.28899999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>113</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C13">
-        <v>0.46600000000000003</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>0.22800000000000001</v>
+        <v>1.4E-2</v>
       </c>
       <c r="E13">
-        <v>0.28899999999999998</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1362,6 +1369,9 @@
       <c r="A15" s="5"/>
     </row>
   </sheetData>
+  <sortState ref="A2:E14">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1370,11 +1380,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B21F2C-9176-F64C-ABF3-5D5E99CB95D5}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:E14"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1394,20 +1407,20 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>58</v>
+      <c r="A2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="C2">
-        <v>6.0000000000000001E-3</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="D2">
-        <v>8.9999999999999993E-3</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E2">
-        <v>8.0000000000000002E-3</v>
+        <v>6.3E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1547,60 +1560,63 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11">
+        <v>1.3029999999999999</v>
+      </c>
+      <c r="D11">
+        <v>1.0329999999999999</v>
+      </c>
+      <c r="E11">
+        <v>0.84699999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>0</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12">
-        <v>1.3029999999999999</v>
-      </c>
-      <c r="D12">
-        <v>1.0329999999999999</v>
-      </c>
-      <c r="E12">
-        <v>0.84699999999999998</v>
-      </c>
-    </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>79</v>
+      <c r="A13" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="C13">
-        <v>5.7000000000000002E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D13">
-        <v>7.0000000000000007E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="E13">
-        <v>6.3E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
     </row>
   </sheetData>
+  <sortState ref="A2:E17">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1609,8 +1625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6106ADFD-11D5-824D-8383-FC720EB1EB02}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:E18"/>
+    <sheetView topLeftCell="A20" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1637,280 +1653,283 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="C2">
-        <v>5.2069999999999999</v>
+        <v>0.60799999999999998</v>
       </c>
       <c r="D2">
-        <v>3.6520000000000001</v>
+        <v>0.68500000000000005</v>
       </c>
       <c r="E2">
-        <v>4.319</v>
+        <v>0.69199999999999995</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="C3">
-        <v>0.41599999999999998</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="D3">
-        <v>0.45400000000000001</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="E3">
-        <v>0.46100000000000002</v>
+        <v>0.151</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C4">
-        <v>0.23300000000000001</v>
+        <v>5.2069999999999999</v>
       </c>
       <c r="D4">
-        <v>0.17799999999999999</v>
+        <v>3.6520000000000001</v>
       </c>
       <c r="E4">
-        <v>2.9000000000000001E-2</v>
+        <v>4.319</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C5">
-        <v>4.9000000000000002E-2</v>
+        <v>0.41599999999999998</v>
       </c>
       <c r="D5">
-        <v>6.6000000000000003E-2</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="E5">
-        <v>7.5999999999999998E-2</v>
+        <v>0.46100000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C6">
-        <v>2.11</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="D6">
-        <v>2.1680000000000001</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="E6">
-        <v>2.1059999999999999</v>
+        <v>2.9000000000000001E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C7">
-        <v>2.9000000000000001E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="D7">
-        <v>1.7999999999999999E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="E7">
-        <v>2.4E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>93</v>
+      <c r="A8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="C8">
-        <v>0.20599999999999999</v>
+        <v>0.47099999999999997</v>
       </c>
       <c r="D8">
-        <v>0.315</v>
+        <v>0.62</v>
       </c>
       <c r="E8">
-        <v>0.374</v>
+        <v>0.41399999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>95</v>
+      <c r="A9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="C9">
-        <v>3.722</v>
+        <v>0.41199999999999998</v>
       </c>
       <c r="D9">
-        <v>3.415</v>
+        <v>0.27700000000000002</v>
       </c>
       <c r="E9">
-        <v>3.3290000000000002</v>
+        <v>0.26500000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>97</v>
+      <c r="A10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C10">
-        <v>2.9990000000000001</v>
+        <v>0.41399999999999998</v>
       </c>
       <c r="D10">
-        <v>2.5670000000000002</v>
+        <v>0.248</v>
       </c>
       <c r="E10">
-        <v>3.4220000000000002</v>
+        <v>0.24299999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="C11">
-        <v>0.60799999999999998</v>
+        <v>4.032</v>
       </c>
       <c r="D11">
-        <v>0.68500000000000005</v>
+        <v>8.5850000000000009</v>
       </c>
       <c r="E11">
-        <v>0.69199999999999995</v>
+        <v>4.2480000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="C12">
-        <v>9.1999999999999998E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="D12">
-        <v>0.10100000000000001</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="E12">
-        <v>0.151</v>
+        <v>3.1E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C13">
-        <v>0.47099999999999997</v>
+        <v>2.11</v>
       </c>
       <c r="D13">
-        <v>0.62</v>
+        <v>2.1680000000000001</v>
       </c>
       <c r="E13">
-        <v>0.41399999999999998</v>
+        <v>2.1059999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C14">
-        <v>0.41199999999999998</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="D14">
-        <v>0.27700000000000002</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="E14">
-        <v>0.26500000000000001</v>
+        <v>2.4E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>107</v>
+      <c r="A15" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="C15">
-        <v>0.41399999999999998</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="D15">
-        <v>0.248</v>
+        <v>0.315</v>
       </c>
       <c r="E15">
-        <v>0.24299999999999999</v>
+        <v>0.374</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>109</v>
+      <c r="A16" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="C16">
-        <v>4.032</v>
+        <v>3.722</v>
       </c>
       <c r="D16">
-        <v>8.5850000000000009</v>
+        <v>3.415</v>
       </c>
       <c r="E16">
-        <v>4.2480000000000002</v>
+        <v>3.3290000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>111</v>
+      <c r="A17" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>97</v>
       </c>
       <c r="C17">
-        <v>2.1000000000000001E-2</v>
+        <v>2.9990000000000001</v>
       </c>
       <c r="D17">
-        <v>3.5000000000000003E-2</v>
+        <v>2.5670000000000002</v>
       </c>
       <c r="E17">
-        <v>3.1E-2</v>
+        <v>3.4220000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
     </row>
   </sheetData>
+  <sortState ref="A2:E17">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>